<commit_message>
v0.7.4 testing now includes BC trials as well as CB trials
Alterations to testing_blocks.xlsx and readme only.
</commit_message>
<xml_diff>
--- a/testing_block.xlsx
+++ b/testing_block.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26819"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26929"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880" tabRatio="500"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="13">
   <si>
     <t>required_response</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>target_category_right</t>
+  </si>
+  <si>
+    <t>bc</t>
   </si>
 </sst>
 </file>
@@ -99,8 +102,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="901">
+  <cellStyleXfs count="915">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1013,7 +1030,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="901">
+  <cellStyles count="915">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1464,6 +1481,13 @@
     <cellStyle name="Followed Hyperlink" xfId="896" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="898" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="900" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="902" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="904" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="906" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="908" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="910" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="912" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="914" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1914,6 +1938,13 @@
     <cellStyle name="Hyperlink" xfId="895" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="897" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="899" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="901" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="903" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="905" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="907" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="909" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="911" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="913" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2241,10 +2272,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -2340,6 +2371,74 @@
         <v>9</v>
       </c>
     </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>